<commit_message>
Updated feature weighting scheme
</commit_message>
<xml_diff>
--- a/Code/Phones/distinctive_features.xlsx
+++ b/Code/Phones/distinctive_features.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/phgeorgis/Documents/School/MSc/Saarland_University/Courses/Thesis/Code/Distance_Measures/Phones/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/phgeorgis/Documents/School/MSc/Saarland_University/Courses/Thesis/Code/Phones/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3001BC6A-6C5D-9B43-929D-109BEE8892B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{275D3169-588F-0E4A-97AB-4ED42DBB0726}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="56">
   <si>
     <t>Feature</t>
   </si>
@@ -193,6 +193,12 @@
   </si>
   <si>
     <t>Features in Node</t>
+  </si>
+  <si>
+    <t>tongue position</t>
+  </si>
+  <si>
+    <t>prosody</t>
   </si>
 </sst>
 </file>
@@ -552,7 +558,7 @@
   <dimension ref="A1:H38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -593,73 +599,73 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C2" t="s">
-        <v>50</v>
+        <v>27</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>43</v>
       </c>
       <c r="D2">
         <f>COUNTIF($B$2:$B$38,B2)</f>
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="E2">
         <f>COUNTIF($C$2:$C$38,C2)</f>
         <v>2</v>
       </c>
       <c r="F2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G2">
         <f>(LOG(IF(B2=C2,D2,D2+E2)))/(F2*F2)</f>
-        <v>7.8454531568956626E-2</v>
+        <v>8.6461250042627072E-2</v>
       </c>
       <c r="H2">
         <f>G2/SUM($G$2:$G$38)</f>
-        <v>8.770378234581171E-3</v>
+        <v>9.7906672907606962E-3</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C3" t="s">
-        <v>50</v>
+        <v>21</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>43</v>
       </c>
       <c r="D3">
         <f>COUNTIF($B$2:$B$38,B3)</f>
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="E3">
         <f>COUNTIF($C$2:$C$38,C3)</f>
         <v>2</v>
       </c>
       <c r="F3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G3">
         <f>(LOG(IF(B3=C3,D3,D3+E3)))/(F3*F3)</f>
-        <v>7.8454531568956626E-2</v>
+        <v>8.6461250042627072E-2</v>
       </c>
       <c r="H3">
         <f>G3/SUM($G$2:$G$38)</f>
-        <v>8.770378234581171E-3</v>
+        <v>9.7906672907606962E-3</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>48</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="D4">
         <f>COUNTIF($B$2:$B$38,B4)</f>
@@ -669,7 +675,7 @@
         <f>COUNTIF($C$2:$C$38,C4)</f>
         <v>2</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="3">
         <v>3</v>
       </c>
       <c r="G4">
@@ -678,18 +684,18 @@
       </c>
       <c r="H4">
         <f>G4/SUM($G$2:$G$38)</f>
-        <v>9.665443797112476E-3</v>
+        <v>9.7906672907606962E-3</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>48</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="D5">
         <f>COUNTIF($B$2:$B$38,B5)</f>
@@ -699,7 +705,7 @@
         <f>COUNTIF($C$2:$C$38,C5)</f>
         <v>2</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="3">
         <v>3</v>
       </c>
       <c r="G5">
@@ -708,7 +714,7 @@
       </c>
       <c r="H5">
         <f>G5/SUM($G$2:$G$38)</f>
-        <v>9.665443797112476E-3</v>
+        <v>9.7906672907606962E-3</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -723,7 +729,7 @@
       </c>
       <c r="D6">
         <f>COUNTIF($B$2:$B$38,B6)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E6">
         <f>COUNTIF($C$2:$C$38,C6)</f>
@@ -734,11 +740,11 @@
       </c>
       <c r="G6">
         <f>(LOG(IF(B6=C6,D6,D6+E6)))/(F6*F6)</f>
-        <v>9.3899782223806308E-2</v>
+        <v>0.10034333188799373</v>
       </c>
       <c r="H6">
         <f>G6/SUM($G$2:$G$38)</f>
-        <v>1.0496992203997109E-2</v>
+        <v>1.1362641378390536E-2</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -753,7 +759,7 @@
       </c>
       <c r="D7">
         <f>COUNTIF($B$2:$B$38,B7)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E7">
         <f>COUNTIF($C$2:$C$38,C7)</f>
@@ -764,11 +770,11 @@
       </c>
       <c r="G7">
         <f>(LOG(IF(B7=C7,D7,D7+E7)))/(F7*F7)</f>
-        <v>0.10034333188799373</v>
+        <v>0.10602694549325832</v>
       </c>
       <c r="H7">
         <f>G7/SUM($G$2:$G$38)</f>
-        <v>1.1217312198241946E-2</v>
+        <v>1.2006240329261033E-2</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
@@ -783,7 +789,7 @@
       </c>
       <c r="D8">
         <f>COUNTIF($B$2:$B$38,B8)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E8">
         <f>COUNTIF($C$2:$C$38,C8)</f>
@@ -794,11 +800,11 @@
       </c>
       <c r="G8">
         <f>(LOG(IF(B8=C8,D8,D8+E8)))/(F8*F8)</f>
-        <v>0.10034333188799373</v>
+        <v>0.10602694549325832</v>
       </c>
       <c r="H8">
         <f>G8/SUM($G$2:$G$38)</f>
-        <v>1.1217312198241946E-2</v>
+        <v>1.2006240329261033E-2</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -813,7 +819,7 @@
       </c>
       <c r="D9">
         <f>COUNTIF($B$2:$B$38,B9)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E9">
         <f>COUNTIF($C$2:$C$38,C9)</f>
@@ -824,11 +830,11 @@
       </c>
       <c r="G9">
         <f>(LOG(IF(B9=C9,D9,D9+E9)))/(F9*F9)</f>
-        <v>0.10602694549325832</v>
+        <v>0.1111111111111111</v>
       </c>
       <c r="H9">
         <f>G9/SUM($G$2:$G$38)</f>
-        <v>1.1852679462063656E-2</v>
+        <v>1.2581959209001728E-2</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -843,7 +849,7 @@
       </c>
       <c r="D10">
         <f>COUNTIF($B$2:$B$38,B10)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E10">
         <f>COUNTIF($C$2:$C$38,C10)</f>
@@ -854,11 +860,11 @@
       </c>
       <c r="G10">
         <f>(LOG(IF(B10=C10,D10,D10+E10)))/(F10*F10)</f>
-        <v>0.10602694549325832</v>
+        <v>0.1111111111111111</v>
       </c>
       <c r="H10" s="3">
         <f>G10/SUM($G$2:$G$38)</f>
-        <v>1.1852679462063656E-2</v>
+        <v>1.2581959209001728E-2</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
@@ -873,7 +879,7 @@
       </c>
       <c r="D11">
         <f>COUNTIF($B$2:$B$38,B11)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E11">
         <f>COUNTIF($C$2:$C$38,C11)</f>
@@ -884,11 +890,11 @@
       </c>
       <c r="G11">
         <f>(LOG(IF(B11=C11,D11,D11+E11)))/(F11*F11)</f>
-        <v>0.10602694549325832</v>
+        <v>0.1111111111111111</v>
       </c>
       <c r="H11">
         <f>G11/SUM($G$2:$G$38)</f>
-        <v>1.1852679462063656E-2</v>
+        <v>1.2581959209001728E-2</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
@@ -903,7 +909,7 @@
       </c>
       <c r="D12">
         <f>COUNTIF($B$2:$B$38,B12)</f>
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E12">
         <f>COUNTIF($C$2:$C$38,C12)</f>
@@ -914,11 +920,11 @@
       </c>
       <c r="G12">
         <f>(LOG(IF(B12=C12,D12,D12+E12)))/(F12*F12)</f>
-        <v>0.13947472278925621</v>
+        <v>0.13671654681980822</v>
       </c>
       <c r="H12">
         <f>G12/SUM($G$2:$G$38)</f>
-        <v>1.5591783528144302E-2</v>
+        <v>1.5481458137541619E-2</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
@@ -933,7 +939,7 @@
       </c>
       <c r="D13">
         <f>COUNTIF($B$2:$B$38,B13)</f>
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E13">
         <f>COUNTIF($C$2:$C$38,C13)</f>
@@ -944,76 +950,76 @@
       </c>
       <c r="G13">
         <f>(LOG(IF(B13=C13,D13,D13+E13)))/(F13*F13)</f>
-        <v>0.13947472278925621</v>
+        <v>0.13671654681980822</v>
       </c>
       <c r="H13">
         <f>G13/SUM($G$2:$G$38)</f>
-        <v>1.5591783528144302E-2</v>
+        <v>1.5481458137541619E-2</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="B14" t="s">
         <v>44</v>
       </c>
       <c r="C14" t="s">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="D14">
         <f>COUNTIF($B$2:$B$38,B14)</f>
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E14">
         <f>COUNTIF($C$2:$C$38,C14)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F14">
         <v>3</v>
       </c>
       <c r="G14">
         <f>(LOG(IF(B14=C14,D14,D14+E14)))/(F14*F14)</f>
-        <v>0.14208373343920322</v>
+        <v>0.13671654681980822</v>
       </c>
       <c r="H14">
         <f>G14/SUM($G$2:$G$38)</f>
-        <v>1.5883443037932769E-2</v>
+        <v>1.5481458137541619E-2</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="B15" t="s">
         <v>44</v>
       </c>
       <c r="C15" t="s">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="D15">
         <f>COUNTIF($B$2:$B$38,B15)</f>
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E15">
         <f>COUNTIF($C$2:$C$38,C15)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F15">
         <v>3</v>
       </c>
       <c r="G15">
         <f>(LOG(IF(B15=C15,D15,D15+E15)))/(F15*F15)</f>
-        <v>0.14208373343920322</v>
+        <v>0.13671654681980822</v>
       </c>
       <c r="H15">
         <f>G15/SUM($G$2:$G$38)</f>
-        <v>1.5883443037932769E-2</v>
+        <v>1.5481458137541619E-2</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="B16" t="s">
         <v>44</v>
@@ -1023,7 +1029,7 @@
       </c>
       <c r="D16">
         <f>COUNTIF($B$2:$B$38,B16)</f>
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E16">
         <f>COUNTIF($C$2:$C$38,C16)</f>
@@ -1034,86 +1040,86 @@
       </c>
       <c r="G16">
         <f>(LOG(IF(B16=C16,D16,D16+E16)))/(F16*F16)</f>
-        <v>0.14208373343920322</v>
+        <v>0.13947472278925621</v>
       </c>
       <c r="H16">
         <f>G16/SUM($G$2:$G$38)</f>
-        <v>1.5883443037932769E-2</v>
+        <v>1.5793787455391211E-2</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="B17" t="s">
         <v>44</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>29</v>
+      <c r="C17" t="s">
+        <v>10</v>
       </c>
       <c r="D17">
         <f>COUNTIF($B$2:$B$38,B17)</f>
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E17">
         <f>COUNTIF($C$2:$C$38,C17)</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F17">
         <v>3</v>
       </c>
       <c r="G17">
         <f>(LOG(IF(B17=C17,D17,D17+E17)))/(F17*F17)</f>
-        <v>0.14691325497043548</v>
+        <v>0.13947472278925621</v>
       </c>
       <c r="H17">
         <f>G17/SUM($G$2:$G$38)</f>
-        <v>1.6423331935028939E-2</v>
+        <v>1.5793787455391211E-2</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>4</v>
+        <v>37</v>
       </c>
       <c r="B18" t="s">
         <v>44</v>
       </c>
-      <c r="C18" s="3" t="s">
-        <v>29</v>
+      <c r="C18" t="s">
+        <v>10</v>
       </c>
       <c r="D18">
         <f>COUNTIF($B$2:$B$38,B18)</f>
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E18">
         <f>COUNTIF($C$2:$C$38,C18)</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F18">
         <v>3</v>
       </c>
       <c r="G18">
         <f>(LOG(IF(B18=C18,D18,D18+E18)))/(F18*F18)</f>
-        <v>0.14691325497043548</v>
+        <v>0.13947472278925621</v>
       </c>
       <c r="H18">
         <f>G18/SUM($G$2:$G$38)</f>
-        <v>1.6423331935028939E-2</v>
+        <v>1.5793787455391211E-2</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="B19" t="s">
         <v>44</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="D19">
         <f>COUNTIF($B$2:$B$38,B19)</f>
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E19">
         <f>COUNTIF($C$2:$C$38,C19)</f>
@@ -1124,26 +1130,26 @@
       </c>
       <c r="G19">
         <f>(LOG(IF(B19=C19,D19,D19+E19)))/(F19*F19)</f>
-        <v>0.14691325497043548</v>
+        <v>0.14455888840710904</v>
       </c>
       <c r="H19">
         <f>G19/SUM($G$2:$G$38)</f>
-        <v>1.6423331935028939E-2</v>
+        <v>1.6369506335131911E-2</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="B20" t="s">
         <v>44</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="D20">
         <f>COUNTIF($B$2:$B$38,B20)</f>
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E20">
         <f>COUNTIF($C$2:$C$38,C20)</f>
@@ -1154,26 +1160,26 @@
       </c>
       <c r="G20">
         <f>(LOG(IF(B20=C20,D20,D20+E20)))/(F20*F20)</f>
-        <v>0.14691325497043548</v>
+        <v>0.14455888840710904</v>
       </c>
       <c r="H20">
         <f>G20/SUM($G$2:$G$38)</f>
-        <v>1.6423331935028939E-2</v>
+        <v>1.6369506335131911E-2</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>13</v>
-      </c>
-      <c r="B21" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B21" t="s">
         <v>44</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="D21">
         <f>COUNTIF($B$2:$B$38,B21)</f>
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E21">
         <f>COUNTIF($C$2:$C$38,C21)</f>
@@ -1184,71 +1190,71 @@
       </c>
       <c r="G21">
         <f>(LOG(IF(B21=C21,D21,D21+E21)))/(F21*F21)</f>
-        <v>0.14691325497043548</v>
+        <v>0.14455888840710904</v>
       </c>
       <c r="H21">
         <f>G21/SUM($G$2:$G$38)</f>
-        <v>1.6423331935028939E-2</v>
+        <v>1.6369506335131911E-2</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>15</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>48</v>
+        <v>23</v>
+      </c>
+      <c r="B22" t="s">
+        <v>44</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="D22">
         <f>COUNTIF($B$2:$B$38,B22)</f>
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="E22">
         <f>COUNTIF($C$2:$C$38,C22)</f>
-        <v>2</v>
-      </c>
-      <c r="F22" s="3">
-        <v>2</v>
+        <v>5</v>
+      </c>
+      <c r="F22">
+        <v>3</v>
       </c>
       <c r="G22">
         <f>(LOG(IF(B22=C22,D22,D22+E22)))/(F22*F22)</f>
-        <v>0.1505149978319906</v>
+        <v>0.14455888840710904</v>
       </c>
       <c r="H22">
         <f>G22/SUM($G$2:$G$38)</f>
-        <v>1.6825968297362919E-2</v>
+        <v>1.6369506335131911E-2</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="D23">
         <f>COUNTIF($B$2:$B$38,B23)</f>
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="E23">
         <f>COUNTIF($C$2:$C$38,C23)</f>
-        <v>2</v>
-      </c>
-      <c r="F23" s="3">
-        <v>2</v>
+        <v>5</v>
+      </c>
+      <c r="F23">
+        <v>3</v>
       </c>
       <c r="G23">
         <f>(LOG(IF(B23=C23,D23,D23+E23)))/(F23*F23)</f>
-        <v>0.1505149978319906</v>
+        <v>0.14455888840710904</v>
       </c>
       <c r="H23">
         <f>G23/SUM($G$2:$G$38)</f>
-        <v>1.6825968297362919E-2</v>
+        <v>1.6369506335131911E-2</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
@@ -1278,7 +1284,7 @@
       </c>
       <c r="H24">
         <f>G24/SUM($G$2:$G$38)</f>
-        <v>2.1747248543503073E-2</v>
+        <v>2.2029001404211563E-2</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
@@ -1308,7 +1314,7 @@
       </c>
       <c r="H25">
         <f>G25/SUM($G$2:$G$38)</f>
-        <v>2.1747248543503073E-2</v>
+        <v>2.2029001404211563E-2</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
@@ -1338,7 +1344,7 @@
       </c>
       <c r="H26">
         <f>G26/SUM($G$2:$G$38)</f>
-        <v>2.1747248543503073E-2</v>
+        <v>2.2029001404211563E-2</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
@@ -1368,7 +1374,7 @@
       </c>
       <c r="H27">
         <f>G27/SUM($G$2:$G$38)</f>
-        <v>2.1747248543503073E-2</v>
+        <v>2.2029001404211563E-2</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
@@ -1398,7 +1404,7 @@
       </c>
       <c r="H28">
         <f>G28/SUM($G$2:$G$38)</f>
-        <v>2.1747248543503073E-2</v>
+        <v>2.2029001404211563E-2</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
@@ -1428,42 +1434,42 @@
       </c>
       <c r="H29">
         <f>G29/SUM($G$2:$G$38)</f>
-        <v>2.1747248543503073E-2</v>
+        <v>2.2029001404211563E-2</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>10</v>
-      </c>
-      <c r="B30" t="s">
-        <v>44</v>
-      </c>
-      <c r="C30" t="s">
-        <v>44</v>
+        <v>33</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>42</v>
       </c>
       <c r="D30">
         <f>COUNTIF($B$2:$B$38,B30)</f>
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="E30">
         <f>COUNTIF($C$2:$C$38,C30)</f>
-        <v>4</v>
-      </c>
-      <c r="F30">
+        <v>1</v>
+      </c>
+      <c r="F30" s="3">
         <v>2</v>
       </c>
       <c r="G30">
         <f>(LOG(IF(B30=C30,D30,D30+E30)))/(F30*F30)</f>
-        <v>0.3010299956639812</v>
+        <v>0.2112745100035642</v>
       </c>
       <c r="H30">
         <f>G30/SUM($G$2:$G$38)</f>
-        <v>3.3651936594725838E-2</v>
+        <v>2.3924225400900053E-2</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="B31" t="s">
         <v>44</v>
@@ -1473,52 +1479,52 @@
       </c>
       <c r="D31">
         <f>COUNTIF($B$2:$B$38,B31)</f>
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E31">
         <f>COUNTIF($C$2:$C$38,C31)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F31">
         <v>2</v>
       </c>
       <c r="G31">
         <f>(LOG(IF(B31=C31,D31,D31+E31)))/(F31*F31)</f>
-        <v>0.3010299956639812</v>
+        <v>0.29402281476392034</v>
       </c>
       <c r="H31">
         <f>G31/SUM($G$2:$G$38)</f>
-        <v>3.3651936594725838E-2</v>
+        <v>3.3294447556879651E-2</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>33</v>
-      </c>
-      <c r="B32" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B32" t="s">
         <v>44</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="C32" t="s">
         <v>44</v>
       </c>
       <c r="D32">
         <f>COUNTIF($B$2:$B$38,B32)</f>
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E32">
         <f>COUNTIF($C$2:$C$38,C32)</f>
-        <v>4</v>
-      </c>
-      <c r="F32" s="3">
+        <v>3</v>
+      </c>
+      <c r="F32">
         <v>2</v>
       </c>
       <c r="G32">
         <f>(LOG(IF(B32=C32,D32,D32+E32)))/(F32*F32)</f>
-        <v>0.3010299956639812</v>
+        <v>0.29402281476392034</v>
       </c>
       <c r="H32">
         <f>G32/SUM($G$2:$G$38)</f>
-        <v>3.3651936594725838E-2</v>
+        <v>3.3294447556879651E-2</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
@@ -1533,22 +1539,22 @@
       </c>
       <c r="D33">
         <f>COUNTIF($B$2:$B$38,B33)</f>
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E33">
         <f>COUNTIF($C$2:$C$38,C33)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F33">
         <v>2</v>
       </c>
       <c r="G33">
         <f>(LOG(IF(B33=C33,D33,D33+E33)))/(F33*F33)</f>
-        <v>0.3010299956639812</v>
+        <v>0.29402281476392034</v>
       </c>
       <c r="H33">
         <f>G33/SUM($G$2:$G$38)</f>
-        <v>3.3651936594725838E-2</v>
+        <v>3.3294447556879651E-2</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
@@ -1578,7 +1584,7 @@
       </c>
       <c r="H34">
         <f>G34/SUM($G$2:$G$38)</f>
-        <v>8.6988994174012291E-2</v>
+        <v>8.8116005616846252E-2</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
@@ -1608,7 +1614,7 @@
       </c>
       <c r="H35">
         <f>G35/SUM($G$2:$G$38)</f>
-        <v>8.6988994174012291E-2</v>
+        <v>8.8116005616846252E-2</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
@@ -1638,7 +1644,7 @@
       </c>
       <c r="H36">
         <f>G36/SUM($G$2:$G$38)</f>
-        <v>8.6988994174012291E-2</v>
+        <v>8.8116005616846252E-2</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
@@ -1668,7 +1674,7 @@
       </c>
       <c r="H37">
         <f>G37/SUM($G$2:$G$38)</f>
-        <v>8.6988994174012291E-2</v>
+        <v>8.8116005616846252E-2</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
@@ -1698,7 +1704,7 @@
       </c>
       <c r="H38">
         <f>G38/SUM($G$2:$G$38)</f>
-        <v>8.6988994174012291E-2</v>
+        <v>8.8116005616846252E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>